<commit_message>
Minor manual adjustments to text & code
</commit_message>
<xml_diff>
--- a/2025-26/MN5813/Week04/assets/data/data.xlsx
+++ b/2025-26/MN5813/Week04/assets/data/data.xlsx
@@ -645,7 +645,7 @@
         <v>-0.4634176928124622</v>
       </c>
       <c r="C12" t="n">
-        <v>-1.918771215299042</v>
+        <v>-1.918771215299041</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
@@ -1671,7 +1671,7 @@
         <v>1.003532897892024</v>
       </c>
       <c r="C69" t="n">
-        <v>1.896792982653947</v>
+        <v>1.896792982653948</v>
       </c>
       <c r="D69" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
fix(Week04): update generated data files in assets/data/
Update data.csv, data.xlsx, people.csv, and people_with_salary.csv with latest generated content. These files were regenerated to ensure consistency with exercise requirements.

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/2025-26/MN5813/Week04/assets/data/data.xlsx
+++ b/2025-26/MN5813/Week04/assets/data/data.xlsx
@@ -645,7 +645,7 @@
         <v>-0.4634176928124622</v>
       </c>
       <c r="C12" t="n">
-        <v>-1.918771215299041</v>
+        <v>-1.918771215299042</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
@@ -1671,7 +1671,7 @@
         <v>1.003532897892024</v>
       </c>
       <c r="C69" t="n">
-        <v>1.896792982653948</v>
+        <v>1.896792982653947</v>
       </c>
       <c r="D69" t="inlineStr">
         <is>

</xml_diff>